<commit_message>
some test cases scenario added
</commit_message>
<xml_diff>
--- a/src/test/java/credentials.xlsx
+++ b/src/test/java/credentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\IdeaProjects\Java\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AC3779-2A97-4C0A-902A-114EEE0A50AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AAEC57-3947-4127-A26E-059482B3A62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58675819-6A4D-405C-9EAD-EF3D6B3DEDD8}"/>
   </bookViews>
@@ -25,12 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>standard_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
@@ -382,16 +391,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A58749-EBED-4E20-86EC-FF02865A5004}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -402,6 +412,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>